<commit_message>
Add new Product ID mapping: UEsDBBQAAAAAAAAAAACkAYS4tQIAALUCAAAaAAAAeGwvX3JlbH...
</commit_message>
<xml_diff>
--- a/Product_ID.xlsx
+++ b/Product_ID.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C449"/>
+  <dimension ref="A1:B450"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -409,9 +409,6 @@
       <c r="B1" t="str">
         <v>Product_ID</v>
       </c>
-      <c r="C1" t="str">
-        <v>LEN</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
@@ -420,9 +417,6 @@
       <c r="B2" t="str">
         <v>010502169116537</v>
       </c>
-      <c r="C2">
-        <v>15</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
@@ -431,9 +425,6 @@
       <c r="B3">
         <v>4895003400249</v>
       </c>
-      <c r="C3">
-        <v>13</v>
-      </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
@@ -442,9 +433,6 @@
       <c r="B4" t="str">
         <v>010489500340016</v>
       </c>
-      <c r="C4">
-        <v>15</v>
-      </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
@@ -453,9 +441,6 @@
       <c r="B5">
         <v>4895003400164</v>
       </c>
-      <c r="C5">
-        <v>13</v>
-      </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
@@ -464,9 +449,6 @@
       <c r="B6" t="str">
         <v>81501070302110454382</v>
       </c>
-      <c r="C6">
-        <v>20</v>
-      </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
@@ -475,9 +457,6 @@
       <c r="B7" t="str">
         <v>6933743787201</v>
       </c>
-      <c r="C7">
-        <v>13</v>
-      </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
@@ -486,9 +465,6 @@
       <c r="B8">
         <v>9313109800152</v>
       </c>
-      <c r="C8">
-        <v>13</v>
-      </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
@@ -497,9 +473,6 @@
       <c r="B9">
         <v>9313109800053</v>
       </c>
-      <c r="C9">
-        <v>13</v>
-      </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
@@ -508,9 +481,6 @@
       <c r="B10" t="str">
         <v>010404772510132</v>
       </c>
-      <c r="C10">
-        <v>15</v>
-      </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
@@ -519,9 +489,6 @@
       <c r="B11" t="str">
         <v>4711916011337</v>
       </c>
-      <c r="C11">
-        <v>13</v>
-      </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
@@ -530,9 +497,6 @@
       <c r="B12" t="str">
         <v>166300000000000</v>
       </c>
-      <c r="C12">
-        <v>15</v>
-      </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
@@ -541,9 +505,6 @@
       <c r="B13" t="str">
         <v>4891768000052</v>
       </c>
-      <c r="C13">
-        <v>13</v>
-      </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
@@ -552,9 +513,6 @@
       <c r="B14" t="str">
         <v>666320000000000</v>
       </c>
-      <c r="C14">
-        <v>15</v>
-      </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
@@ -563,9 +521,6 @@
       <c r="B15" t="str">
         <v>2800941902016</v>
       </c>
-      <c r="C15">
-        <v>13</v>
-      </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
@@ -574,9 +529,6 @@
       <c r="B16" t="str">
         <v>3582910079750</v>
       </c>
-      <c r="C16">
-        <v>13</v>
-      </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
@@ -585,9 +537,6 @@
       <c r="B17" t="str">
         <v>3582910008934</v>
       </c>
-      <c r="C17">
-        <v>13</v>
-      </c>
     </row>
     <row r="18">
       <c r="A18" t="str">
@@ -596,9 +545,6 @@
       <c r="B18" t="str">
         <v>010489326830056</v>
       </c>
-      <c r="C18">
-        <v>15</v>
-      </c>
     </row>
     <row r="19">
       <c r="A19" t="str">
@@ -607,9 +553,6 @@
       <c r="B19" t="str">
         <v>010426009568306</v>
       </c>
-      <c r="C19">
-        <v>15</v>
-      </c>
     </row>
     <row r="20">
       <c r="A20" t="str">
@@ -618,9 +561,6 @@
       <c r="B20">
         <v>4260095683069</v>
       </c>
-      <c r="C20">
-        <v>13</v>
-      </c>
     </row>
     <row r="21">
       <c r="A21" t="str">
@@ -629,9 +569,6 @@
       <c r="B21">
         <v>5010724533819</v>
       </c>
-      <c r="C21">
-        <v>13</v>
-      </c>
     </row>
     <row r="22">
       <c r="A22" t="str">
@@ -640,9 +577,6 @@
       <c r="B22">
         <v>4895103611064</v>
       </c>
-      <c r="C22">
-        <v>13</v>
-      </c>
     </row>
     <row r="23">
       <c r="A23" t="str">
@@ -651,9 +585,6 @@
       <c r="B23" t="str">
         <v>010489510361106</v>
       </c>
-      <c r="C23">
-        <v>15</v>
-      </c>
     </row>
     <row r="24">
       <c r="A24" t="str">
@@ -662,9 +593,6 @@
       <c r="B24">
         <v>5024071230130</v>
       </c>
-      <c r="C24">
-        <v>13</v>
-      </c>
     </row>
     <row r="25">
       <c r="A25" t="str">
@@ -673,9 +601,6 @@
       <c r="B25" t="str">
         <v>010489704258325</v>
       </c>
-      <c r="C25">
-        <v>15</v>
-      </c>
     </row>
     <row r="26">
       <c r="A26" t="str">
@@ -684,9 +609,6 @@
       <c r="B26">
         <v>4897042583259</v>
       </c>
-      <c r="C26">
-        <v>13</v>
-      </c>
     </row>
     <row r="27">
       <c r="A27" t="str">
@@ -695,9 +617,6 @@
       <c r="B27">
         <v>8993430102821</v>
       </c>
-      <c r="C27">
-        <v>13</v>
-      </c>
     </row>
     <row r="28">
       <c r="A28" t="str">
@@ -706,9 +625,6 @@
       <c r="B28" t="str">
         <v>010501412417005</v>
       </c>
-      <c r="C28">
-        <v>15</v>
-      </c>
     </row>
     <row r="29">
       <c r="A29" t="str">
@@ -717,9 +633,6 @@
       <c r="B29">
         <v>5014124170056</v>
       </c>
-      <c r="C29">
-        <v>13</v>
-      </c>
     </row>
     <row r="30">
       <c r="A30" t="str">
@@ -728,9 +641,6 @@
       <c r="B30">
         <v>4897104270189</v>
       </c>
-      <c r="C30">
-        <v>13</v>
-      </c>
     </row>
     <row r="31">
       <c r="A31" t="str">
@@ -739,9 +649,6 @@
       <c r="B31" t="str">
         <v>010498750111670</v>
       </c>
-      <c r="C31">
-        <v>15</v>
-      </c>
     </row>
     <row r="32">
       <c r="A32" t="str">
@@ -750,9 +657,6 @@
       <c r="B32" t="str">
         <v>0801500110813</v>
       </c>
-      <c r="C32">
-        <v>13</v>
-      </c>
     </row>
     <row r="33">
       <c r="A33" t="str">
@@ -761,9 +665,6 @@
       <c r="B33">
         <v>5026468000296</v>
       </c>
-      <c r="C33">
-        <v>13</v>
-      </c>
     </row>
     <row r="34">
       <c r="A34" t="str">
@@ -772,9 +673,6 @@
       <c r="B34">
         <v>6091403218752</v>
       </c>
-      <c r="C34">
-        <v>13</v>
-      </c>
     </row>
     <row r="35">
       <c r="A35" t="str">
@@ -783,9 +681,6 @@
       <c r="B35">
         <v>6091403218028</v>
       </c>
-      <c r="C35">
-        <v>13</v>
-      </c>
     </row>
     <row r="36">
       <c r="A36" t="str">
@@ -794,9 +689,6 @@
       <c r="B36" t="str">
         <v>9329829004343</v>
       </c>
-      <c r="C36">
-        <v>13</v>
-      </c>
     </row>
     <row r="37">
       <c r="A37" t="str">
@@ -805,9 +697,6 @@
       <c r="B37">
         <v>4892018047254</v>
       </c>
-      <c r="C37">
-        <v>13</v>
-      </c>
     </row>
     <row r="38">
       <c r="A38" t="str">
@@ -816,9 +705,6 @@
       <c r="B38">
         <v>4891663004940</v>
       </c>
-      <c r="C38">
-        <v>13</v>
-      </c>
     </row>
     <row r="39">
       <c r="A39" t="str">
@@ -827,9 +713,6 @@
       <c r="B39" t="str">
         <v>010501412417010</v>
       </c>
-      <c r="C39">
-        <v>15</v>
-      </c>
     </row>
     <row r="40">
       <c r="A40" t="str">
@@ -838,9 +721,6 @@
       <c r="B40">
         <v>5014124170100</v>
       </c>
-      <c r="C40">
-        <v>13</v>
-      </c>
     </row>
     <row r="41">
       <c r="A41" t="str">
@@ -849,9 +729,6 @@
       <c r="B41" t="str">
         <v>4713680234516</v>
       </c>
-      <c r="C41">
-        <v>13</v>
-      </c>
     </row>
     <row r="42">
       <c r="A42" t="str">
@@ -860,9 +737,6 @@
       <c r="B42">
         <v>4893776001359</v>
       </c>
-      <c r="C42">
-        <v>13</v>
-      </c>
     </row>
     <row r="43">
       <c r="A43" t="str">
@@ -871,9 +745,6 @@
       <c r="B43" t="str">
         <v>010489377600135</v>
       </c>
-      <c r="C43">
-        <v>15</v>
-      </c>
     </row>
     <row r="44">
       <c r="A44" t="str">
@@ -882,9 +753,6 @@
       <c r="B44" t="str">
         <v>0064642022004</v>
       </c>
-      <c r="C44">
-        <v>13</v>
-      </c>
     </row>
     <row r="45">
       <c r="A45" t="str">
@@ -893,9 +761,6 @@
       <c r="B45">
         <v>8906080480034</v>
       </c>
-      <c r="C45">
-        <v>13</v>
-      </c>
     </row>
     <row r="46">
       <c r="A46" t="str">
@@ -904,9 +769,6 @@
       <c r="B46">
         <v>8906080480034</v>
       </c>
-      <c r="C46">
-        <v>13</v>
-      </c>
     </row>
     <row r="47">
       <c r="A47" t="str">
@@ -915,9 +777,6 @@
       <c r="B47" t="str">
         <v>4895103600327</v>
       </c>
-      <c r="C47">
-        <v>13</v>
-      </c>
     </row>
     <row r="48">
       <c r="A48" t="str">
@@ -926,9 +785,6 @@
       <c r="B48" t="str">
         <v>010489510360032</v>
       </c>
-      <c r="C48">
-        <v>15</v>
-      </c>
     </row>
     <row r="49">
       <c r="A49" t="str">
@@ -937,9 +793,6 @@
       <c r="B49" t="str">
         <v>8853872005954</v>
       </c>
-      <c r="C49">
-        <v>13</v>
-      </c>
     </row>
     <row r="50">
       <c r="A50" t="str">
@@ -948,9 +801,6 @@
       <c r="B50">
         <v>8854927005011</v>
       </c>
-      <c r="C50">
-        <v>13</v>
-      </c>
     </row>
     <row r="51">
       <c r="A51" t="str">
@@ -959,9 +809,6 @@
       <c r="B51">
         <v>4895126673520</v>
       </c>
-      <c r="C51">
-        <v>13</v>
-      </c>
     </row>
     <row r="52">
       <c r="A52" t="str">
@@ -970,9 +817,6 @@
       <c r="B52" t="str">
         <v>010489512667352</v>
       </c>
-      <c r="C52">
-        <v>15</v>
-      </c>
     </row>
     <row r="53">
       <c r="A53" t="str">
@@ -981,9 +825,6 @@
       <c r="B53">
         <v>9350279000180</v>
       </c>
-      <c r="C53">
-        <v>13</v>
-      </c>
     </row>
     <row r="54">
       <c r="A54" t="str">
@@ -992,9 +833,6 @@
       <c r="B54">
         <v>4894281008208</v>
       </c>
-      <c r="C54">
-        <v>13</v>
-      </c>
     </row>
     <row r="55">
       <c r="A55" t="str">
@@ -1003,9 +841,6 @@
       <c r="B55">
         <v>8936106321065</v>
       </c>
-      <c r="C55">
-        <v>13</v>
-      </c>
     </row>
     <row r="56">
       <c r="A56" t="str">
@@ -1014,9 +849,6 @@
       <c r="B56">
         <v>5000223446741</v>
       </c>
-      <c r="C56">
-        <v>13</v>
-      </c>
     </row>
     <row r="57">
       <c r="A57" t="str">
@@ -1025,9 +857,6 @@
       <c r="B57" t="str">
         <v>4895103600556</v>
       </c>
-      <c r="C57">
-        <v>13</v>
-      </c>
     </row>
     <row r="58">
       <c r="A58" t="str">
@@ -1036,9 +865,6 @@
       <c r="B58" t="str">
         <v>010489510360055</v>
       </c>
-      <c r="C58">
-        <v>15</v>
-      </c>
     </row>
     <row r="59">
       <c r="A59" t="str">
@@ -1047,9 +873,6 @@
       <c r="B59">
         <v>9556258002835</v>
       </c>
-      <c r="C59">
-        <v>13</v>
-      </c>
     </row>
     <row r="60">
       <c r="A60" t="str">
@@ -1058,9 +881,6 @@
       <c r="B60">
         <v>4895103607241</v>
       </c>
-      <c r="C60">
-        <v>13</v>
-      </c>
     </row>
     <row r="61">
       <c r="A61" t="str">
@@ -1069,9 +889,6 @@
       <c r="B61" t="str">
         <v>010489510360724</v>
       </c>
-      <c r="C61">
-        <v>15</v>
-      </c>
     </row>
     <row r="62">
       <c r="A62" t="str">
@@ -1080,9 +897,6 @@
       <c r="B62">
         <v>8902346024363</v>
       </c>
-      <c r="C62">
-        <v>13</v>
-      </c>
     </row>
     <row r="63">
       <c r="A63" t="str">
@@ -1091,9 +905,6 @@
       <c r="B63">
         <v>4891034025680</v>
       </c>
-      <c r="C63">
-        <v>13</v>
-      </c>
     </row>
     <row r="64">
       <c r="A64" t="str">
@@ -1102,9 +913,6 @@
       <c r="B64" t="str">
         <v>0798232260049</v>
       </c>
-      <c r="C64">
-        <v>13</v>
-      </c>
     </row>
     <row r="65">
       <c r="A65" t="str">
@@ -1113,9 +921,6 @@
       <c r="B65" t="str">
         <v>010079823226004</v>
       </c>
-      <c r="C65">
-        <v>15</v>
-      </c>
     </row>
     <row r="66">
       <c r="A66" t="str">
@@ -1124,9 +929,6 @@
       <c r="B66">
         <v>8885018070069</v>
       </c>
-      <c r="C66">
-        <v>13</v>
-      </c>
     </row>
     <row r="67">
       <c r="A67" t="str">
@@ -1135,9 +937,6 @@
       <c r="B67" t="str">
         <v>010888501807006</v>
       </c>
-      <c r="C67">
-        <v>15</v>
-      </c>
     </row>
     <row r="68">
       <c r="A68" t="str">
@@ -1146,9 +945,6 @@
       <c r="B68">
         <v>8885018070076</v>
       </c>
-      <c r="C68">
-        <v>13</v>
-      </c>
     </row>
     <row r="69">
       <c r="A69" t="str">
@@ -1157,9 +953,6 @@
       <c r="B69" t="str">
         <v>010888501807007</v>
       </c>
-      <c r="C69">
-        <v>15</v>
-      </c>
     </row>
     <row r="70">
       <c r="A70" t="str">
@@ -1168,9 +961,6 @@
       <c r="B70" t="str">
         <v>4260016651306</v>
       </c>
-      <c r="C70">
-        <v>13</v>
-      </c>
     </row>
     <row r="71">
       <c r="A71" t="str">
@@ -1179,9 +969,6 @@
       <c r="B71" t="str">
         <v>010426001665130</v>
       </c>
-      <c r="C71">
-        <v>15</v>
-      </c>
     </row>
     <row r="72">
       <c r="A72" t="str">
@@ -1190,9 +977,6 @@
       <c r="B72" t="str">
         <v>010005760640702</v>
       </c>
-      <c r="C72">
-        <v>15</v>
-      </c>
     </row>
     <row r="73">
       <c r="A73" t="str">
@@ -1201,9 +985,6 @@
       <c r="B73">
         <v>57606407023</v>
       </c>
-      <c r="C73">
-        <v>11</v>
-      </c>
     </row>
     <row r="74">
       <c r="A74" t="str">
@@ -1212,9 +993,6 @@
       <c r="B74">
         <v>9556492002707</v>
       </c>
-      <c r="C74">
-        <v>13</v>
-      </c>
     </row>
     <row r="75">
       <c r="A75" t="str">
@@ -1223,9 +1001,6 @@
       <c r="B75">
         <v>6432100052995</v>
       </c>
-      <c r="C75">
-        <v>13</v>
-      </c>
     </row>
     <row r="76">
       <c r="A76" t="str">
@@ -1234,9 +1009,6 @@
       <c r="B76">
         <v>4895126695102</v>
       </c>
-      <c r="C76">
-        <v>13</v>
-      </c>
     </row>
     <row r="77">
       <c r="A77" t="str">
@@ -1245,9 +1017,6 @@
       <c r="B77" t="str">
         <v>010489512669510</v>
       </c>
-      <c r="C77">
-        <v>15</v>
-      </c>
     </row>
     <row r="78">
       <c r="A78" t="str">
@@ -1256,9 +1025,6 @@
       <c r="B78">
         <v>4030539913393</v>
       </c>
-      <c r="C78">
-        <v>13</v>
-      </c>
     </row>
     <row r="79">
       <c r="A79" t="str">
@@ -1267,9 +1033,6 @@
       <c r="B79" t="str">
         <v>010403053991338</v>
       </c>
-      <c r="C79">
-        <v>15</v>
-      </c>
     </row>
     <row r="80">
       <c r="A80" t="str">
@@ -1278,9 +1041,6 @@
       <c r="B80" t="str">
         <v>010403053991339</v>
       </c>
-      <c r="C80">
-        <v>15</v>
-      </c>
     </row>
     <row r="81">
       <c r="A81" t="str">
@@ -1289,9 +1049,6 @@
       <c r="B81">
         <v>4895158500290</v>
       </c>
-      <c r="C81">
-        <v>13</v>
-      </c>
     </row>
     <row r="82">
       <c r="A82" t="str">
@@ -1300,9 +1057,6 @@
       <c r="B82">
         <v>4895158500313</v>
       </c>
-      <c r="C82">
-        <v>13</v>
-      </c>
     </row>
     <row r="83">
       <c r="A83" t="str">
@@ -1311,9 +1065,6 @@
       <c r="B83">
         <v>9316626102105</v>
       </c>
-      <c r="C83">
-        <v>13</v>
-      </c>
     </row>
     <row r="84">
       <c r="A84" t="str">
@@ -1322,9 +1073,6 @@
       <c r="B84">
         <v>9555701010083</v>
       </c>
-      <c r="C84">
-        <v>13</v>
-      </c>
     </row>
     <row r="85">
       <c r="A85" t="str">
@@ -1333,9 +1081,6 @@
       <c r="B85">
         <v>114987051142039</v>
       </c>
-      <c r="C85">
-        <v>15</v>
-      </c>
     </row>
     <row r="86">
       <c r="A86" t="str">
@@ -1344,9 +1089,6 @@
       <c r="B86">
         <v>4893268338451</v>
       </c>
-      <c r="C86">
-        <v>13</v>
-      </c>
     </row>
     <row r="87">
       <c r="A87" t="str">
@@ -1355,9 +1097,6 @@
       <c r="B87" t="str">
         <v>0801500110783</v>
       </c>
-      <c r="C87">
-        <v>13</v>
-      </c>
     </row>
     <row r="88">
       <c r="A88" t="str">
@@ -1366,9 +1105,6 @@
       <c r="B88" t="str">
         <v>010489510361122</v>
       </c>
-      <c r="C88">
-        <v>15</v>
-      </c>
     </row>
     <row r="89">
       <c r="A89" t="str">
@@ -1377,9 +1113,6 @@
       <c r="B89">
         <v>4895103611224</v>
       </c>
-      <c r="C89">
-        <v>13</v>
-      </c>
     </row>
     <row r="90">
       <c r="A90" t="str">
@@ -1388,9 +1121,6 @@
       <c r="B90" t="str">
         <v>010366005334604</v>
       </c>
-      <c r="C90">
-        <v>15</v>
-      </c>
     </row>
     <row r="91">
       <c r="A91" t="str">
@@ -1399,9 +1129,6 @@
       <c r="B91">
         <v>3660053346042</v>
       </c>
-      <c r="C91">
-        <v>13</v>
-      </c>
     </row>
     <row r="92">
       <c r="A92" t="str">
@@ -1410,9 +1137,6 @@
       <c r="B92">
         <v>4891663004926</v>
       </c>
-      <c r="C92">
-        <v>13</v>
-      </c>
     </row>
     <row r="93">
       <c r="A93" t="str">
@@ -1421,9 +1145,6 @@
       <c r="B93">
         <v>5603690001941</v>
       </c>
-      <c r="C93">
-        <v>13</v>
-      </c>
     </row>
     <row r="94">
       <c r="A94" t="str">
@@ -1432,9 +1153,6 @@
       <c r="B94">
         <v>4893629900037</v>
       </c>
-      <c r="C94">
-        <v>13</v>
-      </c>
     </row>
     <row r="95">
       <c r="A95" t="str">
@@ -1443,9 +1161,6 @@
       <c r="B95" t="str">
         <v>6091403218738</v>
       </c>
-      <c r="C95">
-        <v>13</v>
-      </c>
     </row>
     <row r="96">
       <c r="A96" t="str">
@@ -1454,9 +1169,6 @@
       <c r="B96" t="str">
         <v>010489510360611</v>
       </c>
-      <c r="C96">
-        <v>15</v>
-      </c>
     </row>
     <row r="97">
       <c r="A97" t="str">
@@ -1465,9 +1177,6 @@
       <c r="B97">
         <v>4895103606114</v>
       </c>
-      <c r="C97">
-        <v>13</v>
-      </c>
     </row>
     <row r="98">
       <c r="A98" t="str">
@@ -1476,9 +1185,6 @@
       <c r="B98" t="str">
         <v>3582910029397</v>
       </c>
-      <c r="C98">
-        <v>13</v>
-      </c>
     </row>
     <row r="99">
       <c r="A99" t="str">
@@ -1487,9 +1193,6 @@
       <c r="B99" t="str">
         <v>3582910029373</v>
       </c>
-      <c r="C99">
-        <v>13</v>
-      </c>
     </row>
     <row r="100">
       <c r="A100" t="str">
@@ -1498,9 +1201,6 @@
       <c r="B100">
         <v>9313109836052</v>
       </c>
-      <c r="C100">
-        <v>13</v>
-      </c>
     </row>
     <row r="101">
       <c r="A101" t="str">
@@ -1509,9 +1209,6 @@
       <c r="B101" t="str">
         <v>012031001911501</v>
       </c>
-      <c r="C101">
-        <v>15</v>
-      </c>
     </row>
     <row r="102">
       <c r="A102" t="str">
@@ -1520,9 +1217,6 @@
       <c r="B102" t="str">
         <v>0310019115016</v>
       </c>
-      <c r="C102">
-        <v>13</v>
-      </c>
     </row>
     <row r="103">
       <c r="A103" t="str">
@@ -1531,9 +1225,6 @@
       <c r="B103" t="str">
         <v>4897042582306</v>
       </c>
-      <c r="C103">
-        <v>13</v>
-      </c>
     </row>
     <row r="104">
       <c r="A104" t="str">
@@ -1542,9 +1233,6 @@
       <c r="B104" t="str">
         <v>010489704258230</v>
       </c>
-      <c r="C104">
-        <v>15</v>
-      </c>
     </row>
     <row r="105">
       <c r="A105" t="str">
@@ -1553,9 +1241,6 @@
       <c r="B105" t="str">
         <v>8435232322415</v>
       </c>
-      <c r="C105">
-        <v>13</v>
-      </c>
     </row>
     <row r="106">
       <c r="A106" t="str">
@@ -1564,9 +1249,6 @@
       <c r="B106" t="str">
         <v>219086100000000</v>
       </c>
-      <c r="C106">
-        <v>15</v>
-      </c>
     </row>
     <row r="107">
       <c r="A107" t="str">
@@ -1575,9 +1257,6 @@
       <c r="B107">
         <v>7640114723971</v>
       </c>
-      <c r="C107">
-        <v>13</v>
-      </c>
     </row>
     <row r="108">
       <c r="A108" t="str">
@@ -1586,9 +1265,6 @@
       <c r="B108" t="str">
         <v>0301320005455</v>
       </c>
-      <c r="C108">
-        <v>13</v>
-      </c>
     </row>
     <row r="109">
       <c r="A109" t="str">
@@ -1597,9 +1273,6 @@
       <c r="B109">
         <v>4260016653621</v>
       </c>
-      <c r="C109">
-        <v>13</v>
-      </c>
     </row>
     <row r="110">
       <c r="A110" t="str">
@@ -1608,9 +1281,6 @@
       <c r="B110" t="str">
         <v>010426001665362</v>
       </c>
-      <c r="C110">
-        <v>15</v>
-      </c>
     </row>
     <row r="111">
       <c r="A111" t="str">
@@ -1619,9 +1289,6 @@
       <c r="B111" t="str">
         <v>011890602596883</v>
       </c>
-      <c r="C111">
-        <v>15</v>
-      </c>
     </row>
     <row r="112">
       <c r="A112" t="str">
@@ -1630,9 +1297,6 @@
       <c r="B112">
         <v>4052682034268</v>
       </c>
-      <c r="C112">
-        <v>13</v>
-      </c>
     </row>
     <row r="113">
       <c r="A113" t="str">
@@ -1641,9 +1305,6 @@
       <c r="B113">
         <v>4030539035903</v>
       </c>
-      <c r="C113">
-        <v>13</v>
-      </c>
     </row>
     <row r="114">
       <c r="A114" t="str">
@@ -1652,9 +1313,6 @@
       <c r="B114" t="str">
         <v>010403053903591</v>
       </c>
-      <c r="C114">
-        <v>15</v>
-      </c>
     </row>
     <row r="115">
       <c r="A115" t="str">
@@ -1663,9 +1321,6 @@
       <c r="B115" t="str">
         <v>010489703879004</v>
       </c>
-      <c r="C115">
-        <v>15</v>
-      </c>
     </row>
     <row r="116">
       <c r="A116" t="str">
@@ -1674,9 +1329,6 @@
       <c r="B116">
         <v>5012617013613</v>
       </c>
-      <c r="C116">
-        <v>13</v>
-      </c>
     </row>
     <row r="117">
       <c r="A117" t="str">
@@ -1685,9 +1337,6 @@
       <c r="B117">
         <v>4029125011537</v>
       </c>
-      <c r="C117">
-        <v>13</v>
-      </c>
     </row>
     <row r="118">
       <c r="A118" t="str">
@@ -1696,9 +1345,6 @@
       <c r="B118" t="str">
         <v>4260016650828</v>
       </c>
-      <c r="C118">
-        <v>13</v>
-      </c>
     </row>
     <row r="119">
       <c r="A119" t="str">
@@ -1707,9 +1353,6 @@
       <c r="B119" t="str">
         <v>010426001665082</v>
       </c>
-      <c r="C119">
-        <v>15</v>
-      </c>
     </row>
     <row r="120">
       <c r="A120" t="str">
@@ -1718,9 +1361,6 @@
       <c r="B120" t="str">
         <v>4987015221216</v>
       </c>
-      <c r="C120">
-        <v>13</v>
-      </c>
     </row>
     <row r="121">
       <c r="A121" t="str">
@@ -1729,9 +1369,6 @@
       <c r="B121" t="str">
         <v>010569052818503</v>
       </c>
-      <c r="C121">
-        <v>15</v>
-      </c>
     </row>
     <row r="122">
       <c r="A122" t="str">
@@ -1740,9 +1377,6 @@
       <c r="B122">
         <v>5690528185034</v>
       </c>
-      <c r="C122">
-        <v>13</v>
-      </c>
     </row>
     <row r="123">
       <c r="A123" t="str">
@@ -1751,9 +1385,6 @@
       <c r="B123" t="str">
         <v>4260016651474</v>
       </c>
-      <c r="C123">
-        <v>13</v>
-      </c>
     </row>
     <row r="124">
       <c r="A124" t="str">
@@ -1762,9 +1393,6 @@
       <c r="B124" t="str">
         <v>010426001665147</v>
       </c>
-      <c r="C124">
-        <v>15</v>
-      </c>
     </row>
     <row r="125">
       <c r="A125" t="str">
@@ -1773,9 +1401,6 @@
       <c r="B125">
         <v>5099602317017</v>
       </c>
-      <c r="C125">
-        <v>13</v>
-      </c>
     </row>
     <row r="126">
       <c r="A126" t="str">
@@ -1784,9 +1409,6 @@
       <c r="B126" t="str">
         <v>010509960200129</v>
       </c>
-      <c r="C126">
-        <v>15</v>
-      </c>
     </row>
     <row r="127">
       <c r="A127" t="str">
@@ -1795,9 +1417,6 @@
       <c r="B127">
         <v>5702191006704</v>
       </c>
-      <c r="C127">
-        <v>13</v>
-      </c>
     </row>
     <row r="128">
       <c r="A128" t="str">
@@ -1806,9 +1425,6 @@
       <c r="B128">
         <v>4891034043271</v>
       </c>
-      <c r="C128">
-        <v>13</v>
-      </c>
     </row>
     <row r="129">
       <c r="A129" t="str">
@@ -1817,9 +1433,6 @@
       <c r="B129">
         <v>9313109808189</v>
       </c>
-      <c r="C129">
-        <v>13</v>
-      </c>
     </row>
     <row r="130">
       <c r="A130" t="str">
@@ -1828,9 +1441,6 @@
       <c r="B130" t="str">
         <v>010403053922252</v>
       </c>
-      <c r="C130">
-        <v>15</v>
-      </c>
     </row>
     <row r="131">
       <c r="A131" t="str">
@@ -1839,9 +1449,6 @@
       <c r="B131">
         <v>4030539222525</v>
       </c>
-      <c r="C131">
-        <v>13</v>
-      </c>
     </row>
     <row r="132">
       <c r="A132" t="str">
@@ -1850,9 +1457,6 @@
       <c r="B132" t="str">
         <v>5012727911793</v>
       </c>
-      <c r="C132">
-        <v>13</v>
-      </c>
     </row>
     <row r="133">
       <c r="A133" t="str">
@@ -1861,9 +1465,6 @@
       <c r="B133" t="str">
         <v>4897078880025</v>
       </c>
-      <c r="C133">
-        <v>13</v>
-      </c>
     </row>
     <row r="134">
       <c r="A134" t="str">
@@ -1872,9 +1473,6 @@
       <c r="B134">
         <v>4895103601355</v>
       </c>
-      <c r="C134">
-        <v>13</v>
-      </c>
     </row>
     <row r="135">
       <c r="A135" t="str">
@@ -1883,9 +1481,6 @@
       <c r="B135" t="str">
         <v>010489510360135</v>
       </c>
-      <c r="C135">
-        <v>15</v>
-      </c>
     </row>
     <row r="136">
       <c r="A136" t="str">
@@ -1894,9 +1489,6 @@
       <c r="B136">
         <v>4895103601256</v>
       </c>
-      <c r="C136">
-        <v>13</v>
-      </c>
     </row>
     <row r="137">
       <c r="A137" t="str">
@@ -1905,9 +1497,6 @@
       <c r="B137" t="str">
         <v>010506033726079</v>
       </c>
-      <c r="C137">
-        <v>15</v>
-      </c>
     </row>
     <row r="138">
       <c r="A138" t="str">
@@ -1916,9 +1505,6 @@
       <c r="B138">
         <v>5060337260794</v>
       </c>
-      <c r="C138">
-        <v>13</v>
-      </c>
     </row>
     <row r="139">
       <c r="A139" t="str">
@@ -1927,9 +1513,6 @@
       <c r="B139" t="str">
         <v>4891609560066</v>
       </c>
-      <c r="C139">
-        <v>13</v>
-      </c>
     </row>
     <row r="140">
       <c r="A140" t="str">
@@ -1938,9 +1521,6 @@
       <c r="B140" t="str">
         <v>955053980000000</v>
       </c>
-      <c r="C140">
-        <v>15</v>
-      </c>
     </row>
     <row r="141">
       <c r="A141" t="str">
@@ -1949,9 +1529,6 @@
       <c r="B141">
         <v>8436035566624</v>
       </c>
-      <c r="C141">
-        <v>13</v>
-      </c>
     </row>
     <row r="142">
       <c r="A142" t="str">
@@ -1960,9 +1537,6 @@
       <c r="B142" t="str">
         <v>4719853700321</v>
       </c>
-      <c r="C142">
-        <v>13</v>
-      </c>
     </row>
     <row r="143">
       <c r="A143" t="str">
@@ -1971,9 +1545,6 @@
       <c r="B143">
         <v>8002660001399</v>
       </c>
-      <c r="C143">
-        <v>13</v>
-      </c>
     </row>
     <row r="144">
       <c r="A144" t="str">
@@ -1982,9 +1553,6 @@
       <c r="B144" t="str">
         <v>5903856931656</v>
       </c>
-      <c r="C144">
-        <v>13</v>
-      </c>
     </row>
     <row r="145">
       <c r="A145" t="str">
@@ -1993,9 +1561,6 @@
       <c r="B145">
         <v>3800714000597</v>
       </c>
-      <c r="C145">
-        <v>13</v>
-      </c>
     </row>
     <row r="146">
       <c r="A146" t="str">
@@ -2004,9 +1569,6 @@
       <c r="B146" t="str">
         <v>010405268205580</v>
       </c>
-      <c r="C146">
-        <v>15</v>
-      </c>
     </row>
     <row r="147">
       <c r="A147" t="str">
@@ -2015,9 +1577,6 @@
       <c r="B147" t="str">
         <v>101048970387900</v>
       </c>
-      <c r="C147">
-        <v>15</v>
-      </c>
     </row>
     <row r="148">
       <c r="A148" t="str">
@@ -2026,9 +1585,6 @@
       <c r="B148" t="str">
         <v>6091403221653</v>
       </c>
-      <c r="C148">
-        <v>13</v>
-      </c>
     </row>
     <row r="149">
       <c r="A149" t="str">
@@ -2037,9 +1593,6 @@
       <c r="B149" t="str">
         <v>6091403218424</v>
       </c>
-      <c r="C149">
-        <v>13</v>
-      </c>
     </row>
     <row r="150">
       <c r="A150" t="str">
@@ -2048,9 +1601,6 @@
       <c r="B150">
         <v>9316795006617</v>
       </c>
-      <c r="C150">
-        <v>13</v>
-      </c>
     </row>
     <row r="151">
       <c r="A151" t="str">
@@ -2059,9 +1609,6 @@
       <c r="B151">
         <v>6091403218042</v>
       </c>
-      <c r="C151">
-        <v>13</v>
-      </c>
     </row>
     <row r="152">
       <c r="A152" t="str">
@@ -2070,9 +1617,6 @@
       <c r="B152" t="str">
         <v>4897042583716</v>
       </c>
-      <c r="C152">
-        <v>13</v>
-      </c>
     </row>
     <row r="153">
       <c r="A153" t="str">
@@ -2081,9 +1625,6 @@
       <c r="B153" t="str">
         <v>010489704258371</v>
       </c>
-      <c r="C153">
-        <v>15</v>
-      </c>
     </row>
     <row r="154">
       <c r="A154" t="str">
@@ -2092,9 +1633,6 @@
       <c r="B154" t="str">
         <v>010489326835315</v>
       </c>
-      <c r="C154">
-        <v>15</v>
-      </c>
     </row>
     <row r="155">
       <c r="A155" t="str">
@@ -2103,9 +1641,6 @@
       <c r="B155" t="str">
         <v>010501412417429</v>
       </c>
-      <c r="C155">
-        <v>15</v>
-      </c>
     </row>
     <row r="156">
       <c r="A156" t="str">
@@ -2114,9 +1649,6 @@
       <c r="B156" t="str">
         <v>7613036951586</v>
       </c>
-      <c r="C156">
-        <v>13</v>
-      </c>
     </row>
     <row r="157">
       <c r="A157" t="str">
@@ -2125,9 +1657,6 @@
       <c r="B157">
         <v>4893629900105</v>
       </c>
-      <c r="C157">
-        <v>13</v>
-      </c>
     </row>
     <row r="158">
       <c r="A158" t="str">
@@ -2136,9 +1665,6 @@
       <c r="B158">
         <v>5413760229225</v>
       </c>
-      <c r="C158">
-        <v>13</v>
-      </c>
     </row>
     <row r="159">
       <c r="A159" t="str">
@@ -2147,9 +1673,6 @@
       <c r="B159">
         <v>4899338800422</v>
       </c>
-      <c r="C159">
-        <v>13</v>
-      </c>
     </row>
     <row r="160">
       <c r="A160" t="str">
@@ -2158,9 +1681,6 @@
       <c r="B160" t="str">
         <v>4891663000065</v>
       </c>
-      <c r="C160">
-        <v>13</v>
-      </c>
     </row>
     <row r="161">
       <c r="A161" t="str">
@@ -2169,9 +1689,6 @@
       <c r="B161" t="str">
         <v>0801500110721</v>
       </c>
-      <c r="C161">
-        <v>13</v>
-      </c>
     </row>
     <row r="162">
       <c r="A162" t="str">
@@ -2180,9 +1697,6 @@
       <c r="B162" t="str">
         <v>011080150011072</v>
       </c>
-      <c r="C162">
-        <v>15</v>
-      </c>
     </row>
     <row r="163">
       <c r="A163" t="str">
@@ -2191,9 +1705,6 @@
       <c r="B163">
         <v>4715718227330</v>
       </c>
-      <c r="C163">
-        <v>13</v>
-      </c>
     </row>
     <row r="164">
       <c r="A164" t="str">
@@ -2202,9 +1713,6 @@
       <c r="B164">
         <v>4715718227033</v>
       </c>
-      <c r="C164">
-        <v>13</v>
-      </c>
     </row>
     <row r="165">
       <c r="A165" t="str">
@@ -2213,9 +1721,6 @@
       <c r="B165" t="str">
         <v>3582910080077</v>
       </c>
-      <c r="C165">
-        <v>13</v>
-      </c>
     </row>
     <row r="166">
       <c r="A166" t="str">
@@ -2224,9 +1729,6 @@
       <c r="B166">
         <v>5000456014069</v>
       </c>
-      <c r="C166">
-        <v>13</v>
-      </c>
     </row>
     <row r="167">
       <c r="A167" t="str">
@@ -2235,9 +1737,6 @@
       <c r="B167">
         <v>3582910082699</v>
       </c>
-      <c r="C167">
-        <v>13</v>
-      </c>
     </row>
     <row r="168">
       <c r="A168" t="str">
@@ -2246,9 +1745,6 @@
       <c r="B168">
         <v>4895158502898</v>
       </c>
-      <c r="C168">
-        <v>13</v>
-      </c>
     </row>
     <row r="169">
       <c r="A169" t="str">
@@ -2257,9 +1753,6 @@
       <c r="B169" t="str">
         <v>010489377600662</v>
       </c>
-      <c r="C169">
-        <v>15</v>
-      </c>
     </row>
     <row r="170">
       <c r="A170" t="str">
@@ -2268,9 +1761,6 @@
       <c r="B170">
         <v>4893776006620</v>
       </c>
-      <c r="C170">
-        <v>13</v>
-      </c>
     </row>
     <row r="171">
       <c r="A171" t="str">
@@ -2279,9 +1769,6 @@
       <c r="B171">
         <v>4987084302663</v>
       </c>
-      <c r="C171">
-        <v>13</v>
-      </c>
     </row>
     <row r="172">
       <c r="A172" t="str">
@@ -2290,9 +1777,6 @@
       <c r="B172">
         <v>4260016650705</v>
       </c>
-      <c r="C172">
-        <v>13</v>
-      </c>
     </row>
     <row r="173">
       <c r="A173" t="str">
@@ -2301,9 +1785,6 @@
       <c r="B173" t="str">
         <v>010426001665070</v>
       </c>
-      <c r="C173">
-        <v>15</v>
-      </c>
     </row>
     <row r="174">
       <c r="A174" t="str">
@@ -2312,9 +1793,6 @@
       <c r="B174">
         <v>4897002622257</v>
       </c>
-      <c r="C174">
-        <v>13</v>
-      </c>
     </row>
     <row r="175">
       <c r="A175" t="str">
@@ -2323,9 +1801,6 @@
       <c r="B175" t="str">
         <v>4260016653676</v>
       </c>
-      <c r="C175">
-        <v>13</v>
-      </c>
     </row>
     <row r="176">
       <c r="A176" t="str">
@@ -2334,9 +1809,6 @@
       <c r="B176" t="str">
         <v>010426001665367</v>
       </c>
-      <c r="C176">
-        <v>15</v>
-      </c>
     </row>
     <row r="177">
       <c r="A177" t="str">
@@ -2345,9 +1817,6 @@
       <c r="B177">
         <v>5702191023268</v>
       </c>
-      <c r="C177">
-        <v>13</v>
-      </c>
     </row>
     <row r="178">
       <c r="A178" t="str">
@@ -2356,9 +1825,6 @@
       <c r="B178">
         <v>3700567700012</v>
       </c>
-      <c r="C178">
-        <v>13</v>
-      </c>
     </row>
     <row r="179">
       <c r="A179" t="str">
@@ -2367,9 +1833,6 @@
       <c r="B179" t="str">
         <v>010030409302401</v>
       </c>
-      <c r="C179">
-        <v>15</v>
-      </c>
     </row>
     <row r="180">
       <c r="A180" t="str">
@@ -2378,9 +1841,6 @@
       <c r="B180">
         <v>100304093024012</v>
       </c>
-      <c r="C180">
-        <v>15</v>
-      </c>
     </row>
     <row r="181">
       <c r="A181" t="str">
@@ -2389,9 +1849,6 @@
       <c r="B181">
         <v>7612098000362</v>
       </c>
-      <c r="C181">
-        <v>13</v>
-      </c>
     </row>
     <row r="182">
       <c r="A182" t="str">
@@ -2400,9 +1857,6 @@
       <c r="B182">
         <v>5997001380932</v>
       </c>
-      <c r="C182">
-        <v>13</v>
-      </c>
     </row>
     <row r="183">
       <c r="A183" t="str">
@@ -2411,9 +1865,6 @@
       <c r="B183">
         <v>4897056490260</v>
       </c>
-      <c r="C183">
-        <v>13</v>
-      </c>
     </row>
     <row r="184">
       <c r="A184" t="str">
@@ -2422,9 +1873,6 @@
       <c r="B184" t="str">
         <v>4893776001939</v>
       </c>
-      <c r="C184">
-        <v>13</v>
-      </c>
     </row>
     <row r="185">
       <c r="A185" t="str">
@@ -2433,9 +1881,6 @@
       <c r="B185" t="str">
         <v>010489704258025</v>
       </c>
-      <c r="C185">
-        <v>15</v>
-      </c>
     </row>
     <row r="186">
       <c r="A186" t="str">
@@ -2444,9 +1889,6 @@
       <c r="B186" t="str">
         <v>010426001665685</v>
       </c>
-      <c r="C186">
-        <v>15</v>
-      </c>
     </row>
     <row r="187">
       <c r="A187" t="str">
@@ -2455,9 +1897,6 @@
       <c r="B187">
         <v>4260016656851</v>
       </c>
-      <c r="C187">
-        <v>13</v>
-      </c>
     </row>
     <row r="188">
       <c r="A188" t="str">
@@ -2466,9 +1905,6 @@
       <c r="B188">
         <v>4052682064906</v>
       </c>
-      <c r="C188">
-        <v>13</v>
-      </c>
     </row>
     <row r="189">
       <c r="A189" t="str">
@@ -2477,9 +1913,6 @@
       <c r="B189" t="str">
         <v>010489704258301</v>
       </c>
-      <c r="C189">
-        <v>15</v>
-      </c>
     </row>
     <row r="190">
       <c r="A190" t="str">
@@ -2488,9 +1921,6 @@
       <c r="B190">
         <v>4897042583013</v>
       </c>
-      <c r="C190">
-        <v>13</v>
-      </c>
     </row>
     <row r="191">
       <c r="A191" t="str">
@@ -2499,9 +1929,6 @@
       <c r="B191">
         <v>4897010454758</v>
       </c>
-      <c r="C191">
-        <v>13</v>
-      </c>
     </row>
     <row r="192">
       <c r="A192" t="str">
@@ -2510,9 +1937,6 @@
       <c r="B192" t="str">
         <v>011890112704053</v>
       </c>
-      <c r="C192">
-        <v>15</v>
-      </c>
     </row>
     <row r="193">
       <c r="A193" t="str">
@@ -2521,9 +1945,6 @@
       <c r="B193" t="str">
         <v>010489326836746</v>
       </c>
-      <c r="C193">
-        <v>15</v>
-      </c>
     </row>
     <row r="194">
       <c r="A194" t="str">
@@ -2532,9 +1953,6 @@
       <c r="B194" t="str">
         <v>17213V01R01</v>
       </c>
-      <c r="C194">
-        <v>11</v>
-      </c>
     </row>
     <row r="195">
       <c r="A195" t="str">
@@ -2543,9 +1961,6 @@
       <c r="B195">
         <v>9340404001229</v>
       </c>
-      <c r="C195">
-        <v>13</v>
-      </c>
     </row>
     <row r="196">
       <c r="A196" t="str">
@@ -2554,9 +1969,6 @@
       <c r="B196" t="str">
         <v>4891663133084</v>
       </c>
-      <c r="C196">
-        <v>13</v>
-      </c>
     </row>
     <row r="197">
       <c r="A197" t="str">
@@ -2565,9 +1977,6 @@
       <c r="B197" t="str">
         <v>3582910013624</v>
       </c>
-      <c r="C197">
-        <v>13</v>
-      </c>
     </row>
     <row r="198">
       <c r="A198" t="str">
@@ -2576,9 +1985,6 @@
       <c r="B198" t="str">
         <v>010501412417026</v>
       </c>
-      <c r="C198">
-        <v>15</v>
-      </c>
     </row>
     <row r="199">
       <c r="A199" t="str">
@@ -2587,9 +1993,6 @@
       <c r="B199">
         <v>5014124170261</v>
       </c>
-      <c r="C199">
-        <v>13</v>
-      </c>
     </row>
     <row r="200">
       <c r="A200" t="str">
@@ -2598,9 +2001,6 @@
       <c r="B200">
         <v>6927924801107</v>
       </c>
-      <c r="C200">
-        <v>13</v>
-      </c>
     </row>
     <row r="201">
       <c r="A201" t="str">
@@ -2609,9 +2009,6 @@
       <c r="B201" t="str">
         <v>010121000117085</v>
       </c>
-      <c r="C201">
-        <v>15</v>
-      </c>
     </row>
     <row r="202">
       <c r="A202" t="str">
@@ -2620,9 +2017,6 @@
       <c r="B202" t="str">
         <v>9313109827159</v>
       </c>
-      <c r="C202">
-        <v>13</v>
-      </c>
     </row>
     <row r="203">
       <c r="A203" t="str">
@@ -2631,9 +2025,6 @@
       <c r="B203">
         <v>9313109827159</v>
       </c>
-      <c r="C203">
-        <v>13</v>
-      </c>
     </row>
     <row r="204">
       <c r="A204" t="str">
@@ -2642,9 +2033,6 @@
       <c r="B204" t="str">
         <v>156900000000000</v>
       </c>
-      <c r="C204">
-        <v>15</v>
-      </c>
     </row>
     <row r="205">
       <c r="A205" t="str">
@@ -2653,9 +2041,6 @@
       <c r="B205" t="str">
         <v>666320000000000</v>
       </c>
-      <c r="C205">
-        <v>15</v>
-      </c>
     </row>
     <row r="206">
       <c r="A206" t="str">
@@ -2664,9 +2049,6 @@
       <c r="B206" t="str">
         <v>5027519001804</v>
       </c>
-      <c r="C206">
-        <v>13</v>
-      </c>
     </row>
     <row r="207">
       <c r="A207" t="str">
@@ -2675,9 +2057,6 @@
       <c r="B207" t="str">
         <v>0801500110806</v>
       </c>
-      <c r="C207">
-        <v>13</v>
-      </c>
     </row>
     <row r="208">
       <c r="A208" t="str">
@@ -2686,9 +2065,6 @@
       <c r="B208" t="str">
         <v>010121000117085</v>
       </c>
-      <c r="C208">
-        <v>15</v>
-      </c>
     </row>
     <row r="209">
       <c r="A209" t="str">
@@ -2697,9 +2073,6 @@
       <c r="B209" t="str">
         <v>5036376224639</v>
       </c>
-      <c r="C209">
-        <v>13</v>
-      </c>
     </row>
     <row r="210">
       <c r="A210" t="str">
@@ -2708,9 +2081,6 @@
       <c r="B210" t="str">
         <v>010489501181637</v>
       </c>
-      <c r="C210">
-        <v>15</v>
-      </c>
     </row>
     <row r="211">
       <c r="A211" t="str">
@@ -2719,9 +2089,6 @@
       <c r="B211" t="str">
         <v>4260095681843</v>
       </c>
-      <c r="C211">
-        <v>13</v>
-      </c>
     </row>
     <row r="212">
       <c r="A212" t="str">
@@ -2730,9 +2097,6 @@
       <c r="B212" t="str">
         <v>5060499390506</v>
       </c>
-      <c r="C212">
-        <v>13</v>
-      </c>
     </row>
     <row r="213">
       <c r="A213" t="str">
@@ -2741,9 +2105,6 @@
       <c r="B213">
         <v>4893629900075</v>
       </c>
-      <c r="C213">
-        <v>13</v>
-      </c>
     </row>
     <row r="214">
       <c r="A214" t="str">
@@ -2752,9 +2113,6 @@
       <c r="B214">
         <v>4893629900082</v>
       </c>
-      <c r="C214">
-        <v>13</v>
-      </c>
     </row>
     <row r="215">
       <c r="A215" t="str">
@@ -2763,9 +2121,6 @@
       <c r="B215">
         <v>4893629900068</v>
       </c>
-      <c r="C215">
-        <v>13</v>
-      </c>
     </row>
     <row r="216">
       <c r="A216" t="str">
@@ -2774,9 +2129,6 @@
       <c r="B216">
         <v>8901175029570</v>
       </c>
-      <c r="C216">
-        <v>13</v>
-      </c>
     </row>
     <row r="217">
       <c r="A217" t="str">
@@ -2785,9 +2137,6 @@
       <c r="B217" t="str">
         <v>011890117502957</v>
       </c>
-      <c r="C217">
-        <v>15</v>
-      </c>
     </row>
     <row r="218">
       <c r="A218" t="str">
@@ -2796,9 +2145,6 @@
       <c r="B218">
         <v>3582910052647</v>
       </c>
-      <c r="C218">
-        <v>13</v>
-      </c>
     </row>
     <row r="219">
       <c r="A219" t="str">
@@ -2807,9 +2153,6 @@
       <c r="B219">
         <v>3582910052654</v>
       </c>
-      <c r="C219">
-        <v>13</v>
-      </c>
     </row>
     <row r="220">
       <c r="A220" t="str">
@@ -2818,9 +2161,6 @@
       <c r="B220" t="str">
         <v>0300870402035</v>
       </c>
-      <c r="C220">
-        <v>13</v>
-      </c>
     </row>
     <row r="221">
       <c r="A221" t="str">
@@ -2829,9 +2169,6 @@
       <c r="B221">
         <v>3665585003012</v>
       </c>
-      <c r="C221">
-        <v>13</v>
-      </c>
     </row>
     <row r="222">
       <c r="A222" t="str">
@@ -2840,9 +2177,6 @@
       <c r="B222" t="str">
         <v>750943860000000</v>
       </c>
-      <c r="C222">
-        <v>15</v>
-      </c>
     </row>
     <row r="223">
       <c r="A223" t="str">
@@ -2851,9 +2185,6 @@
       <c r="B223" t="str">
         <v>010890409382110</v>
       </c>
-      <c r="C223">
-        <v>15</v>
-      </c>
     </row>
     <row r="224">
       <c r="A224" t="str">
@@ -2862,9 +2193,6 @@
       <c r="B224" t="str">
         <v>010403053991231</v>
       </c>
-      <c r="C224">
-        <v>15</v>
-      </c>
     </row>
     <row r="225">
       <c r="A225" t="str">
@@ -2873,9 +2201,6 @@
       <c r="B225" t="str">
         <v>4030539912310</v>
       </c>
-      <c r="C225">
-        <v>13</v>
-      </c>
     </row>
     <row r="226">
       <c r="A226" t="str">
@@ -2884,9 +2209,6 @@
       <c r="B226" t="str">
         <v>010030338070948</v>
       </c>
-      <c r="C226">
-        <v>15</v>
-      </c>
     </row>
     <row r="227">
       <c r="A227" t="str">
@@ -2895,9 +2217,6 @@
       <c r="B227" t="str">
         <v>010030338070548</v>
       </c>
-      <c r="C227">
-        <v>15</v>
-      </c>
     </row>
     <row r="228">
       <c r="A228" t="str">
@@ -2906,9 +2225,6 @@
       <c r="B228">
         <v>5291043001160</v>
       </c>
-      <c r="C228">
-        <v>13</v>
-      </c>
     </row>
     <row r="229">
       <c r="A229" t="str">
@@ -2917,9 +2233,6 @@
       <c r="B229">
         <v>5291043000354</v>
       </c>
-      <c r="C229">
-        <v>13</v>
-      </c>
     </row>
     <row r="230">
       <c r="A230" t="str">
@@ -2928,9 +2241,6 @@
       <c r="B230">
         <v>5291043000385</v>
       </c>
-      <c r="C230">
-        <v>13</v>
-      </c>
     </row>
     <row r="231">
       <c r="A231" t="str">
@@ -2939,9 +2249,6 @@
       <c r="B231">
         <v>4897046660185</v>
       </c>
-      <c r="C231">
-        <v>13</v>
-      </c>
     </row>
     <row r="232">
       <c r="A232" t="str">
@@ -2950,9 +2257,6 @@
       <c r="B232">
         <v>4897000501202</v>
       </c>
-      <c r="C232">
-        <v>13</v>
-      </c>
     </row>
     <row r="233">
       <c r="A233" t="str">
@@ -2961,9 +2265,6 @@
       <c r="B233">
         <v>9331134000118</v>
       </c>
-      <c r="C233">
-        <v>13</v>
-      </c>
     </row>
     <row r="234">
       <c r="A234" t="str">
@@ -2972,9 +2273,6 @@
       <c r="B234">
         <v>4893629900198</v>
       </c>
-      <c r="C234">
-        <v>13</v>
-      </c>
     </row>
     <row r="235">
       <c r="A235" t="str">
@@ -2983,9 +2281,6 @@
       <c r="B235" t="str">
         <v>011501272791359</v>
       </c>
-      <c r="C235">
-        <v>15</v>
-      </c>
     </row>
     <row r="236">
       <c r="A236" t="str">
@@ -2994,9 +2289,6 @@
       <c r="B236" t="str">
         <v>010404772512352</v>
       </c>
-      <c r="C236">
-        <v>15</v>
-      </c>
     </row>
     <row r="237">
       <c r="A237" t="str">
@@ -3005,9 +2297,6 @@
       <c r="B237">
         <v>3664798045482</v>
       </c>
-      <c r="C237">
-        <v>13</v>
-      </c>
     </row>
     <row r="238">
       <c r="A238" t="str">
@@ -3016,9 +2305,6 @@
       <c r="B238" t="str">
         <v>010366479804548</v>
       </c>
-      <c r="C238">
-        <v>15</v>
-      </c>
     </row>
     <row r="239">
       <c r="A239" t="str">
@@ -3027,9 +2313,6 @@
       <c r="B239" t="str">
         <v>010489377600635</v>
       </c>
-      <c r="C239">
-        <v>15</v>
-      </c>
     </row>
     <row r="240">
       <c r="A240" t="str">
@@ -3038,9 +2321,6 @@
       <c r="B240" t="str">
         <v>4893776006354</v>
       </c>
-      <c r="C240">
-        <v>13</v>
-      </c>
     </row>
     <row r="241">
       <c r="A241" t="str">
@@ -3049,9 +2329,6 @@
       <c r="B241" t="str">
         <v>9300670501243</v>
       </c>
-      <c r="C241">
-        <v>13</v>
-      </c>
     </row>
     <row r="242">
       <c r="A242" t="str">
@@ -3060,9 +2337,6 @@
       <c r="B242">
         <v>8054083002279</v>
       </c>
-      <c r="C242">
-        <v>13</v>
-      </c>
     </row>
     <row r="243">
       <c r="A243" t="str">
@@ -3071,9 +2345,6 @@
       <c r="B243">
         <v>4030539071475</v>
       </c>
-      <c r="C243">
-        <v>13</v>
-      </c>
     </row>
     <row r="244">
       <c r="A244" t="str">
@@ -3082,9 +2353,6 @@
       <c r="B244" t="str">
         <v>010403053905797</v>
       </c>
-      <c r="C244">
-        <v>15</v>
-      </c>
     </row>
     <row r="245">
       <c r="A245" t="str">
@@ -3093,9 +2361,6 @@
       <c r="B245" t="str">
         <v>010405268205372</v>
       </c>
-      <c r="C245">
-        <v>15</v>
-      </c>
     </row>
     <row r="246">
       <c r="A246" t="str">
@@ -3104,9 +2369,6 @@
       <c r="B246">
         <v>9556492000130</v>
       </c>
-      <c r="C246">
-        <v>13</v>
-      </c>
     </row>
     <row r="247">
       <c r="A247" t="str">
@@ -3115,9 +2377,6 @@
       <c r="B247" t="str">
         <v>013070441101761</v>
       </c>
-      <c r="C247">
-        <v>15</v>
-      </c>
     </row>
     <row r="248">
       <c r="A248" t="str">
@@ -3126,9 +2385,6 @@
       <c r="B248" t="str">
         <v>010489510360390</v>
       </c>
-      <c r="C248">
-        <v>15</v>
-      </c>
     </row>
     <row r="249">
       <c r="A249" t="str">
@@ -3137,9 +2393,6 @@
       <c r="B249">
         <v>4895103603908</v>
       </c>
-      <c r="C249">
-        <v>13</v>
-      </c>
     </row>
     <row r="250">
       <c r="A250" t="str">
@@ -3148,9 +2401,6 @@
       <c r="B250" t="str">
         <v>010415001676515</v>
       </c>
-      <c r="C250">
-        <v>15</v>
-      </c>
     </row>
     <row r="251">
       <c r="A251" t="str">
@@ -3159,9 +2409,6 @@
       <c r="B251" t="str">
         <v>0801500110615</v>
       </c>
-      <c r="C251">
-        <v>13</v>
-      </c>
     </row>
     <row r="252">
       <c r="A252" t="str">
@@ -3170,9 +2417,6 @@
       <c r="B252">
         <v>110801500110612</v>
       </c>
-      <c r="C252">
-        <v>15</v>
-      </c>
     </row>
     <row r="253">
       <c r="A253" t="str">
@@ -3181,9 +2425,6 @@
       <c r="B253" t="str">
         <v>010339113587001</v>
       </c>
-      <c r="C253">
-        <v>15</v>
-      </c>
     </row>
     <row r="254">
       <c r="A254" t="str">
@@ -3192,9 +2433,6 @@
       <c r="B254">
         <v>4893645241459</v>
       </c>
-      <c r="C254">
-        <v>13</v>
-      </c>
     </row>
     <row r="255">
       <c r="A255" t="str">
@@ -3203,9 +2441,6 @@
       <c r="B255">
         <v>6923878313697</v>
       </c>
-      <c r="C255">
-        <v>13</v>
-      </c>
     </row>
     <row r="256">
       <c r="A256" t="str">
@@ -3214,9 +2449,6 @@
       <c r="B256">
         <v>4893629900839</v>
       </c>
-      <c r="C256">
-        <v>13</v>
-      </c>
     </row>
     <row r="257">
       <c r="A257" t="str">
@@ -3225,9 +2457,6 @@
       <c r="B257">
         <v>4893629900822</v>
       </c>
-      <c r="C257">
-        <v>13</v>
-      </c>
     </row>
     <row r="258">
       <c r="A258" t="str">
@@ -3236,9 +2465,6 @@
       <c r="B258" t="str">
         <v>010426001665081</v>
       </c>
-      <c r="C258">
-        <v>15</v>
-      </c>
     </row>
     <row r="259">
       <c r="A259" t="str">
@@ -3247,9 +2473,6 @@
       <c r="B259" t="str">
         <v>4260016650811</v>
       </c>
-      <c r="C259">
-        <v>13</v>
-      </c>
     </row>
     <row r="260">
       <c r="A260" t="str">
@@ -3258,9 +2481,6 @@
       <c r="B260">
         <v>4823002246827</v>
       </c>
-      <c r="C260">
-        <v>13</v>
-      </c>
     </row>
     <row r="261">
       <c r="A261" t="str">
@@ -3269,9 +2489,6 @@
       <c r="B261">
         <v>5713844000000</v>
       </c>
-      <c r="C261">
-        <v>13</v>
-      </c>
     </row>
     <row r="262">
       <c r="A262" t="str">
@@ -3280,9 +2497,6 @@
       <c r="B262">
         <v>4895103601003</v>
       </c>
-      <c r="C262">
-        <v>13</v>
-      </c>
     </row>
     <row r="263">
       <c r="A263" t="str">
@@ -3291,9 +2505,6 @@
       <c r="B263" t="str">
         <v>010489510360100</v>
       </c>
-      <c r="C263">
-        <v>15</v>
-      </c>
     </row>
     <row r="264">
       <c r="A264" t="str">
@@ -3302,9 +2513,6 @@
       <c r="B264">
         <v>4711914315215</v>
       </c>
-      <c r="C264">
-        <v>13</v>
-      </c>
     </row>
     <row r="265">
       <c r="A265" t="str">
@@ -3313,9 +2521,6 @@
       <c r="B265">
         <v>3582910055112</v>
       </c>
-      <c r="C265">
-        <v>13</v>
-      </c>
     </row>
     <row r="266">
       <c r="A266" t="str">
@@ -3324,9 +2529,6 @@
       <c r="B266">
         <v>3582910005810</v>
       </c>
-      <c r="C266">
-        <v>13</v>
-      </c>
     </row>
     <row r="267">
       <c r="A267" t="str">
@@ -3335,9 +2537,6 @@
       <c r="B267" t="str">
         <v>3700567700029</v>
       </c>
-      <c r="C267">
-        <v>13</v>
-      </c>
     </row>
     <row r="268">
       <c r="A268" t="str">
@@ -3346,9 +2545,6 @@
       <c r="B268">
         <v>8435373701452</v>
       </c>
-      <c r="C268">
-        <v>13</v>
-      </c>
     </row>
     <row r="269">
       <c r="A269" t="str">
@@ -3357,9 +2553,6 @@
       <c r="B269" t="str">
         <v>011030409114405</v>
       </c>
-      <c r="C269">
-        <v>15</v>
-      </c>
     </row>
     <row r="270">
       <c r="A270" t="str">
@@ -3368,9 +2561,6 @@
       <c r="B270">
         <v>4891034025703</v>
       </c>
-      <c r="C270">
-        <v>13</v>
-      </c>
     </row>
     <row r="271">
       <c r="A271" t="str">
@@ -3379,9 +2569,6 @@
       <c r="B271">
         <v>4891034025710</v>
       </c>
-      <c r="C271">
-        <v>13</v>
-      </c>
     </row>
     <row r="272">
       <c r="A272" t="str">
@@ -3390,9 +2577,6 @@
       <c r="B272" t="str">
         <v>4895103600723</v>
       </c>
-      <c r="C272">
-        <v>13</v>
-      </c>
     </row>
     <row r="273">
       <c r="A273" t="str">
@@ -3401,9 +2585,6 @@
       <c r="B273" t="str">
         <v>010880646601621</v>
       </c>
-      <c r="C273">
-        <v>15</v>
-      </c>
     </row>
     <row r="274">
       <c r="A274" t="str">
@@ -3412,9 +2593,6 @@
       <c r="B274" t="str">
         <v>010489506611886</v>
       </c>
-      <c r="C274">
-        <v>15</v>
-      </c>
     </row>
     <row r="275">
       <c r="A275" t="str">
@@ -3423,9 +2601,6 @@
       <c r="B275" t="str">
         <v>020404772510132</v>
       </c>
-      <c r="C275">
-        <v>15</v>
-      </c>
     </row>
     <row r="276">
       <c r="A276" t="str">
@@ -3434,9 +2609,6 @@
       <c r="B276" t="str">
         <v>010489704258412</v>
       </c>
-      <c r="C276">
-        <v>15</v>
-      </c>
     </row>
     <row r="277">
       <c r="A277" t="str">
@@ -3445,9 +2617,6 @@
       <c r="B277" t="str">
         <v>244100000000000</v>
       </c>
-      <c r="C277">
-        <v>15</v>
-      </c>
     </row>
     <row r="278">
       <c r="A278" t="str">
@@ -3456,9 +2625,6 @@
       <c r="B278" t="str">
         <v>010121000113568</v>
       </c>
-      <c r="C278">
-        <v>15</v>
-      </c>
     </row>
     <row r="279">
       <c r="A279" t="str">
@@ -3467,9 +2633,6 @@
       <c r="B279" t="str">
         <v>1210001135680</v>
       </c>
-      <c r="C279">
-        <v>13</v>
-      </c>
     </row>
     <row r="280">
       <c r="A280" t="str">
@@ -3478,9 +2641,6 @@
       <c r="B280" t="str">
         <v>172130101000000</v>
       </c>
-      <c r="C280">
-        <v>15</v>
-      </c>
     </row>
     <row r="449">
       <c r="A449" t="str">
@@ -3490,9 +2650,17 @@
         <v>4550583435059</v>
       </c>
     </row>
+    <row r="450">
+      <c r="A450" t="str">
+        <v>MOME02</v>
+      </c>
+      <c r="B450" t="str">
+        <v>9314839004889</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C449"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:B450"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>